<commit_message>
Bug fixes - colorSchemes
</commit_message>
<xml_diff>
--- a/references/代码样式.xlsx
+++ b/references/代码样式.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projects\__Pinned\Paradox-Language-Support\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1B4A32-8559-4012-AD9F-BB18B4732AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BA5C41-99E3-446A-B717-D20B2C32041B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{CF4CB8EA-B1DB-4511-B4F0-540424C937D8}"/>
+    <workbookView xWindow="38820" yWindow="4815" windowWidth="39600" windowHeight="17235" xr2:uid="{CF4CB8EA-B1DB-4511-B4F0-540424C937D8}"/>
   </bookViews>
   <sheets>
     <sheet name="自定义的代码样式" sheetId="1" r:id="rId1"/>
@@ -352,48 +352,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-      </rPr>
-      <t>蓝色字体：已检查过的键名</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-      </rPr>
-      <t>灰色背景色：继承的样式，不写入到</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>xml</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-      </rPr>
-      <t>配置文件中</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PARADOX_LOCALISATION.VARIABLE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -411,6 +369,14 @@
   </si>
   <si>
     <t>PARADOX_SCRIPT.MACRO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蓝色字体：已检查过的键名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>灰色背景色：继承的样式，不需要到xml配置文件中覆盖</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -732,7 +698,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -807,6 +773,15 @@
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1125,7 +1100,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1526,10 +1501,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>15</v>
@@ -1540,29 +1515,29 @@
       <c r="E14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="25" t="s">
         <v>40</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" s="26" t="s">
         <v>39</v>
       </c>
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>15</v>
@@ -1573,19 +1548,19 @@
       <c r="E15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="25" t="s">
         <v>40</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="J15" s="8" t="s">
+      <c r="J15" s="26" t="s">
         <v>39</v>
       </c>
       <c r="K15" s="3"/>
@@ -1671,7 +1646,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>23</v>
@@ -1704,7 +1679,7 @@
     </row>
     <row r="20" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B20" s="22" t="s">
         <v>65</v>
@@ -1745,13 +1720,13 @@
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:11" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>79</v>
+      <c r="A22" s="27" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>80</v>
+      <c r="A23" s="27" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
`PARADOX_SCRIPT.DIRECTIVE` 改为参照 jsp/freemarker directive name
</commit_message>
<xml_diff>
--- a/references/代码样式.xlsx
+++ b/references/代码样式.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projects\__Pinned\Paradox-Language-Support\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BA5C41-99E3-446A-B717-D20B2C32041B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2014B2-F833-463B-8548-EC95EC90DCD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38820" yWindow="4815" windowWidth="39600" windowHeight="17235" xr2:uid="{CF4CB8EA-B1DB-4511-B4F0-540424C937D8}"/>
+    <workbookView xWindow="38865" yWindow="5625" windowWidth="39600" windowHeight="17235" xr2:uid="{CF4CB8EA-B1DB-4511-B4F0-540424C937D8}"/>
   </bookViews>
   <sheets>
     <sheet name="自定义的代码样式" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="88">
   <si>
     <t>PARADOX_SCRIPT.CONDITION_PARAMETER</t>
   </si>
@@ -360,23 +360,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DEFAULT_TAG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PARADOX_SCRIPT.INLINE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PARADOX_SCRIPT.MACRO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>蓝色字体：已检查过的键名</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>灰色背景色：继承的样式，不需要到xml配置文件中覆盖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PARADOX_SCRIPT.DIRECTIVE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KEYWORD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JSP directive name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#CC7832, bold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#CF8E6D, bold</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -479,7 +487,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -692,13 +700,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -726,9 +760,6 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -774,14 +805,23 @@
     <xf numFmtId="49" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1097,94 +1137,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467F33A7-5074-4910-85C9-08134893D597}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="51" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.25" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.25" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.75" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.75" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.5" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="13" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1216,7 +1256,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>48</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1248,7 +1288,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>63</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1280,7 +1320,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="4"/>
@@ -1310,7 +1350,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>64</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1342,7 +1382,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="15" t="s">
         <v>62</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1374,7 +1414,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="15" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1390,7 +1430,7 @@
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="15" t="s">
         <v>68</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1422,7 +1462,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1454,7 +1494,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -1487,7 +1527,7 @@
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="16"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -1500,233 +1540,200 @@
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
-        <v>82</v>
+      <c r="A14" s="15" t="s">
+        <v>83</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="25" t="s">
+      <c r="G14" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J14" s="26" t="s">
+      <c r="H14" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="J14" s="29" t="s">
         <v>39</v>
       </c>
       <c r="K14" s="3"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="H15" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J15" s="26" t="s">
-        <v>39</v>
-      </c>
+    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="16"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="27"/>
       <c r="K15" s="3"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="17"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="9"/>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="16" t="s">
-        <v>41</v>
+      <c r="A17" s="15" t="s">
+        <v>7</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="K17" s="3"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>44</v>
+      <c r="A18" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>30</v>
       </c>
       <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H19" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="I19" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="J19" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="K19" s="3"/>
-    </row>
-    <row r="20" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="21" t="s">
+      <c r="A19" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B19" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C19" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D19" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E19" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="F20" s="22" t="s">
+      <c r="F19" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="22" t="s">
+      <c r="G19" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H20" s="22" t="s">
+      <c r="H19" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="I20" s="22" t="s">
+      <c r="I19" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="J20" s="23" t="s">
+      <c r="J19" s="22" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="24" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="22" spans="1:11" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="27" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="27" t="s">
-        <v>85</v>
+      <c r="A22" s="24" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>